<commit_message>
Tests were added for annotation icon on delivery panel
git-tfs-id: [https://dev.azure.com/TR-Legal-Cobalt]$/Cobalt QED Testing/PLPlusANZ;C819605
</commit_message>
<xml_diff>
--- a/src/test/resources/CobaltUsers.xlsx
+++ b/src/test/resources/CobaltUsers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="58">
   <si>
     <t>UserName</t>
   </si>
@@ -178,6 +178,15 @@
   </si>
   <si>
     <t>librarian</t>
+  </si>
+  <si>
+    <t>auAnnotationUser1</t>
+  </si>
+  <si>
+    <t>ANZ annotation user</t>
+  </si>
+  <si>
+    <t>auannotationuser1@mailinator.com</t>
   </si>
   <si>
     <t>Y</t>
@@ -584,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,6 +933,41 @@
         <v>9</v>
       </c>
       <c r="G17" s="6"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Test was added for sharing annotation
git-tfs-id: [https://dev.azure.com/TR-Legal-Cobalt]$/Cobalt QED Testing/PLPlusANZ;C820035
</commit_message>
<xml_diff>
--- a/src/test/resources/CobaltUsers.xlsx
+++ b/src/test/resources/CobaltUsers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="62">
   <si>
     <t>UserName</t>
   </si>
@@ -187,6 +187,18 @@
   </si>
   <si>
     <t>auannotationuser1@mailinator.com</t>
+  </si>
+  <si>
+    <t>shareAnnotationUser1</t>
+  </si>
+  <si>
+    <t>shareannotationuser1@mailinator.com</t>
+  </si>
+  <si>
+    <t>myShareAnnotationUser</t>
+  </si>
+  <si>
+    <t>myShareAnnotationUser@mailinator.com</t>
   </si>
   <si>
     <t>Y</t>
@@ -593,15 +605,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="24.0" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="27.42578125" collapsed="true"/>
@@ -961,13 +973,38 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
+      <c r="A20" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="E20" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
+      <c r="G20" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="7" t="s">
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -979,9 +1016,11 @@
     <hyperlink ref="G8" r:id="rId6"/>
     <hyperlink ref="G10" r:id="rId7"/>
     <hyperlink ref="G11" r:id="rId8"/>
+    <hyperlink ref="G20" r:id="rId9"/>
+    <hyperlink ref="G21" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Test was added for annotation for group
git-tfs-id: [https://dev.azure.com/TR-Legal-Cobalt]$/Cobalt QED Testing/PLPlusANZ;C820287
</commit_message>
<xml_diff>
--- a/src/test/resources/CobaltUsers.xlsx
+++ b/src/test/resources/CobaltUsers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="64">
   <si>
     <t>UserName</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>myShareAnnotationUser@mailinator.com</t>
+  </si>
+  <si>
+    <t>userForAnnotationGroup</t>
+  </si>
+  <si>
+    <t>userforannotationgroup@mailinator.com</t>
   </si>
   <si>
     <t>Y</t>
@@ -605,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,6 +1010,23 @@
       <c r="F21" s="6"/>
       <c r="G21" s="7" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="7" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added users and changed documents
git-tfs-id: [https://dev.azure.com/TR-Legal-Cobalt]$/Cobalt QED Testing/PLPlusANZ;C821152
</commit_message>
<xml_diff>
--- a/src/test/resources/CobaltUsers.xlsx
+++ b/src/test/resources/CobaltUsers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="67">
   <si>
     <t>UserName</t>
   </si>
@@ -207,15 +207,23 @@
     <t>userforannotationgroup@mailinator.com</t>
   </si>
   <si>
-    <t>Y</t>
+    <t>auAnnotationUser2</t>
+  </si>
+  <si>
+    <t>auAnnotationUser3</t>
+  </si>
+  <si>
+    <t>auannotationuser2@mailinator.com</t>
+  </si>
+  <si>
+    <t>auannotationuser3@mailinator.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -611,20 +619,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="27.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="35.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="40.7109375" collapsed="true"/>
+    <col min="1" max="1" width="24" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="35.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="40.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -980,7 +988,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>13</v>
@@ -992,12 +1000,12 @@
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="7" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>13</v>
@@ -1009,12 +1017,12 @@
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="7" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>13</v>
@@ -1026,6 +1034,40 @@
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" s="7" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1039,11 +1081,13 @@
     <hyperlink ref="G8" r:id="rId6"/>
     <hyperlink ref="G10" r:id="rId7"/>
     <hyperlink ref="G11" r:id="rId8"/>
-    <hyperlink ref="G20" r:id="rId9"/>
-    <hyperlink ref="G21" r:id="rId10"/>
+    <hyperlink ref="G22" r:id="rId9"/>
+    <hyperlink ref="G23" r:id="rId10"/>
+    <hyperlink ref="G20" r:id="rId11"/>
+    <hyperlink ref="G21" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 
@@ -1057,8 +1101,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="28.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="1" max="1" width="28.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Kostya - update Browser users
git-tfs-id: [https://dev.azure.com/TR-Legal-Cobalt]$/Cobalt QED Testing/PLPlusANZ;C824465
</commit_message>
<xml_diff>
--- a/src/test/resources/CobaltUsers.xlsx
+++ b/src/test/resources/CobaltUsers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="90">
   <si>
     <t>UserName</t>
   </si>
@@ -217,13 +217,83 @@
   </si>
   <si>
     <t>auannotationuser3@mailinator.com</t>
+  </si>
+  <si>
+    <t>AUtestuser1</t>
+  </si>
+  <si>
+    <t>AUtestuser1@mailinator.com</t>
+  </si>
+  <si>
+    <t>AUtestuser2@mailinator.com</t>
+  </si>
+  <si>
+    <t>AUtestuser2</t>
+  </si>
+  <si>
+    <t>AUtestuser3@mailinator.com</t>
+  </si>
+  <si>
+    <t>AUtestuser3</t>
+  </si>
+  <si>
+    <t>thomsonreuters</t>
+  </si>
+  <si>
+    <t>answer</t>
+  </si>
+  <si>
+    <t>AUtestuser4@mailinator.com</t>
+  </si>
+  <si>
+    <t>AUtestuser4</t>
+  </si>
+  <si>
+    <t>AUtestuser5</t>
+  </si>
+  <si>
+    <t>AUtestuser5@mailinator.com</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>AUtestuser6</t>
+  </si>
+  <si>
+    <t>AUtestuser6@mailinator.com</t>
+  </si>
+  <si>
+    <t>AUtestuser7</t>
+  </si>
+  <si>
+    <t>AUtestuser7@mailinator.com</t>
+  </si>
+  <si>
+    <t>AUtestuser8</t>
+  </si>
+  <si>
+    <t>AUtestuser8@mailinator.com</t>
+  </si>
+  <si>
+    <t>AUtestuser9</t>
+  </si>
+  <si>
+    <t>AUtestuser9@mailinator.com</t>
+  </si>
+  <si>
+    <t>AUtestuser10</t>
+  </si>
+  <si>
+    <t>AUtestuser10@mailinator.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,7 +332,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -298,12 +368,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -314,6 +395,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -619,23 +701,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="35.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="35.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="40.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="15.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -657,8 +740,11 @@
       <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -681,7 +767,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -700,7 +786,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -719,7 +805,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -738,7 +824,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -757,7 +843,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>24</v>
       </c>
@@ -774,11 +860,11 @@
       <c r="F7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>25</v>
       </c>
@@ -797,7 +883,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>33</v>
       </c>
@@ -816,7 +902,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>35</v>
       </c>
@@ -835,7 +921,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>38</v>
       </c>
@@ -854,7 +940,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>42</v>
       </c>
@@ -869,7 +955,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>44</v>
       </c>
@@ -884,7 +970,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>46</v>
       </c>
@@ -901,7 +987,7 @@
       </c>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>48</v>
       </c>
@@ -918,7 +1004,7 @@
       </c>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>50</v>
       </c>
@@ -939,7 +1025,7 @@
       </c>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>52</v>
       </c>
@@ -960,114 +1046,298 @@
       </c>
       <c r="G17" s="6"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
+      <c r="D18" s="6" t="s">
+        <v>79</v>
+      </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>54</v>
+      <c r="G18" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="D19" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="6"/>
       <c r="F19" s="6"/>
-      <c r="G19" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>63</v>
+      <c r="G19" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>64</v>
+        <v>71</v>
+      </c>
+      <c r="H20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>76</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
-      <c r="E21" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>57</v>
+        <v>75</v>
+      </c>
+      <c r="H21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
-      <c r="E22" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>59</v>
+        <v>78</v>
+      </c>
+      <c r="H22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>80</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
-      <c r="E23" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="E23" s="6"/>
       <c r="F23" s="6"/>
       <c r="G23" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>61</v>
+        <v>81</v>
+      </c>
+      <c r="H23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>82</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
-      <c r="E24" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="H26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="H27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F30" s="6"/>
+      <c r="G30" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31" s="6"/>
+      <c r="G31" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32" s="6"/>
+      <c r="G32" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" s="6"/>
+      <c r="G33" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" s="6"/>
+      <c r="G34" s="7" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1081,13 +1351,23 @@
     <hyperlink ref="G8" r:id="rId6"/>
     <hyperlink ref="G10" r:id="rId7"/>
     <hyperlink ref="G11" r:id="rId8"/>
-    <hyperlink ref="G22" r:id="rId9"/>
-    <hyperlink ref="G23" r:id="rId10"/>
-    <hyperlink ref="G20" r:id="rId11"/>
-    <hyperlink ref="G21" r:id="rId12"/>
+    <hyperlink ref="G32" r:id="rId9"/>
+    <hyperlink ref="G33" r:id="rId10"/>
+    <hyperlink ref="G30" r:id="rId11"/>
+    <hyperlink ref="G31" r:id="rId12"/>
+    <hyperlink ref="G18" r:id="rId13"/>
+    <hyperlink ref="G19" r:id="rId14"/>
+    <hyperlink ref="G20" r:id="rId15"/>
+    <hyperlink ref="G21" r:id="rId16"/>
+    <hyperlink ref="G22" r:id="rId17"/>
+    <hyperlink ref="G23" r:id="rId18"/>
+    <hyperlink ref="G24" r:id="rId19"/>
+    <hyperlink ref="G25" r:id="rId20"/>
+    <hyperlink ref="G26" r:id="rId21"/>
+    <hyperlink ref="G27" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
 
@@ -1101,8 +1381,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Kostya - update user name for LegalUpdates
git-tfs-id: [https://dev.azure.com/TR-Legal-Cobalt]$/Cobalt QED Testing/PLPlusANZ;C824512
</commit_message>
<xml_diff>
--- a/src/test/resources/CobaltUsers.xlsx
+++ b/src/test/resources/CobaltUsers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="94">
   <si>
     <t>UserName</t>
   </si>
@@ -286,14 +286,25 @@
   </si>
   <si>
     <t>AUtestuser10@mailinator.com</t>
+  </si>
+  <si>
+    <t>AUtestuser11</t>
+  </si>
+  <si>
+    <t>AUtestuser11@mailinator.com</t>
+  </si>
+  <si>
+    <t>AUtestuser12</t>
+  </si>
+  <si>
+    <t>AUtestuser12@mailinator.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -701,21 +712,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="27.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="35.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="40.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="1" max="1" width="24" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="35.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="40.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1231,51 +1242,53 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
+      <c r="A28" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
+      <c r="G28" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="H28" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>54</v>
+      <c r="A29" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
-      <c r="E29" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="E29" s="6"/>
       <c r="F29" s="6"/>
-      <c r="G29" s="6" t="s">
-        <v>56</v>
+      <c r="G29" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="H29" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
-      <c r="E30" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="E30" s="6"/>
       <c r="F30" s="6"/>
-      <c r="G30" s="7" t="s">
-        <v>65</v>
-      </c>
+      <c r="G30" s="6"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>13</v>
@@ -1286,13 +1299,13 @@
         <v>55</v>
       </c>
       <c r="F31" s="6"/>
-      <c r="G31" s="7" t="s">
-        <v>66</v>
+      <c r="G31" s="6" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>13</v>
@@ -1304,12 +1317,12 @@
       </c>
       <c r="F32" s="6"/>
       <c r="G32" s="7" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>13</v>
@@ -1321,12 +1334,12 @@
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="7" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>13</v>
@@ -1338,6 +1351,40 @@
       </c>
       <c r="F34" s="6"/>
       <c r="G34" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F35" s="6"/>
+      <c r="G35" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F36" s="6"/>
+      <c r="G36" s="7" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1351,10 +1398,10 @@
     <hyperlink ref="G8" r:id="rId6"/>
     <hyperlink ref="G10" r:id="rId7"/>
     <hyperlink ref="G11" r:id="rId8"/>
-    <hyperlink ref="G32" r:id="rId9"/>
-    <hyperlink ref="G33" r:id="rId10"/>
-    <hyperlink ref="G30" r:id="rId11"/>
-    <hyperlink ref="G31" r:id="rId12"/>
+    <hyperlink ref="G34" r:id="rId9"/>
+    <hyperlink ref="G35" r:id="rId10"/>
+    <hyperlink ref="G32" r:id="rId11"/>
+    <hyperlink ref="G33" r:id="rId12"/>
     <hyperlink ref="G18" r:id="rId13"/>
     <hyperlink ref="G19" r:id="rId14"/>
     <hyperlink ref="G20" r:id="rId15"/>
@@ -1365,9 +1412,11 @@
     <hyperlink ref="G25" r:id="rId20"/>
     <hyperlink ref="G26" r:id="rId21"/>
     <hyperlink ref="G27" r:id="rId22"/>
+    <hyperlink ref="G28" r:id="rId23"/>
+    <hyperlink ref="G29" r:id="rId24"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId25"/>
 </worksheet>
 </file>
 
@@ -1381,8 +1430,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="28.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="1" max="1" width="28.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Kostya - add screenshots for report fix
git-tfs-id: [https://dev.azure.com/TR-Legal-Cobalt]$/Cobalt QED Testing/PLPlusANZ;C824523
</commit_message>
<xml_diff>
--- a/src/test/resources/CobaltUsers.xlsx
+++ b/src/test/resources/CobaltUsers.xlsx
@@ -304,7 +304,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -720,13 +721,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="35.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="35.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="40.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="15.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1430,8 +1431,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed test issue with name of list docs in delivery
git-tfs-id: [https://dev.azure.com/TR-Legal-Cobalt]$/Cobalt QED Testing/PLPlusANZ;C854584
</commit_message>
<xml_diff>
--- a/src/test/resources/CobaltUsers.xlsx
+++ b/src/test/resources/CobaltUsers.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Emails" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="90">
   <si>
     <t>UserName</t>
   </si>
@@ -280,12 +280,18 @@
   </si>
   <si>
     <t>AUtestuser13@mailinator.com</t>
+  </si>
+  <si>
+    <t>TestUserProd1</t>
+  </si>
+  <si>
+    <t>TestUserProd1@mailinator.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
   <fonts count="3">
     <font>
@@ -697,7 +703,7 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1220,13 +1226,22 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
+      <c r="A28" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
+      <c r="G28" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H28" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
@@ -1354,9 +1369,10 @@
     <hyperlink ref="G25" r:id="rId20"/>
     <hyperlink ref="G26" r:id="rId21"/>
     <hyperlink ref="G27" r:id="rId22"/>
+    <hyperlink ref="G28" r:id="rId23"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId24"/>
 </worksheet>
 </file>
 

</xml_diff>